<commit_message>
added mixed refunds jul
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -126,13 +126,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1635"/>
+  <dimension ref="A1:B1641"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1596" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1630" activeCellId="0" sqref="B1630"/>
+      <selection pane="topLeft" activeCell="A1636" activeCellId="0" sqref="A1636"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -13212,6 +13212,54 @@
       </c>
       <c r="B1635" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="1636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1636" s="0" t="n">
+        <v>3848908</v>
+      </c>
+      <c r="B1636" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1637" s="0" t="n">
+        <v>3848116</v>
+      </c>
+      <c r="B1637" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1638" s="0" t="n">
+        <v>3870270</v>
+      </c>
+      <c r="B1638" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1639" s="0" t="n">
+        <v>3872722</v>
+      </c>
+      <c r="B1639" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1640" s="0" t="n">
+        <v>3872506</v>
+      </c>
+      <c r="B1640" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1641" s="0" t="n">
+        <v>3894926</v>
+      </c>
+      <c r="B1641" s="1" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ozon fixes 14.10.2025 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD410F-A3CB-064E-8915-355C176ABF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C88B7-A0AE-8C45-A13C-5D270E4682F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3175"/>
+  <dimension ref="A1:B3176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3163" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3178" sqref="B3178"/>
+    <sheetView tabSelected="1" topLeftCell="A3156" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3182" sqref="C3182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25802,6 +25802,14 @@
         <v>4174602</v>
       </c>
       <c r="B3175" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3176" spans="1:2" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3176" s="1">
+        <v>4274436</v>
+      </c>
+      <c r="B3176" s="2">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 14.10.2025 part 4
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C88B7-A0AE-8C45-A13C-5D270E4682F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30667554-55BF-D642-9CF7-1ACD4EDC948D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3176"/>
+  <dimension ref="A1:B3179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3156" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3182" sqref="C3182"/>
+      <selection activeCell="E3184" sqref="E3184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25810,6 +25810,30 @@
         <v>4274436</v>
       </c>
       <c r="B3176" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3177" spans="1:2" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3177" s="1">
+        <v>4228763</v>
+      </c>
+      <c r="B3177" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3178" spans="1:2" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3178" s="1">
+        <v>4290222</v>
+      </c>
+      <c r="B3178" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3179" spans="1:2" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3179" s="1">
+        <v>4290223</v>
+      </c>
+      <c r="B3179" s="2">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 14.10.2025 part 6
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30667554-55BF-D642-9CF7-1ACD4EDC948D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBCE759-2A72-8A42-8097-54A786F28AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="7820" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3179"/>
+  <dimension ref="A1:B3182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3156" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3184" sqref="E3184"/>
+      <selection activeCell="E3179" sqref="E3179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25834,6 +25834,30 @@
         <v>4290223</v>
       </c>
       <c r="B3179" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3180" spans="1:2" ht="14" x14ac:dyDescent="0.2">
+      <c r="A3180" s="1">
+        <v>4268338</v>
+      </c>
+      <c r="B3180" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3181" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3181">
+        <v>4263634</v>
+      </c>
+      <c r="B3181" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3182" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3182">
+        <v>4250014</v>
+      </c>
+      <c r="B3182" s="2">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 16.09.2025 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBCE759-2A72-8A42-8097-54A786F28AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4714DD03-DD1B-A84D-8AFF-DAD97F007B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="7820" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="6840" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -54,6 +54,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -79,10 +86,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3182"/>
+  <dimension ref="A1:B3197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3156" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3179" sqref="E3179"/>
+    <sheetView tabSelected="1" topLeftCell="A3173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E3194" sqref="E3194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25858,6 +25866,126 @@
         <v>4250014</v>
       </c>
       <c r="B3182" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3183" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3183">
+        <v>4107268</v>
+      </c>
+      <c r="B3183" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3184" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3184">
+        <v>4303051</v>
+      </c>
+      <c r="B3184" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3185" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3185">
+        <v>4303055</v>
+      </c>
+      <c r="B3185" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3186" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3186">
+        <v>4131598</v>
+      </c>
+      <c r="B3186" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3187" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3187">
+        <v>4303157</v>
+      </c>
+      <c r="B3187" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3188" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3188">
+        <v>4303158</v>
+      </c>
+      <c r="B3188" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3189" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3189">
+        <v>4130775</v>
+      </c>
+      <c r="B3189" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3190" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3190">
+        <v>4303164</v>
+      </c>
+      <c r="B3190" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3191" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3191">
+        <v>4303165</v>
+      </c>
+      <c r="B3191" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3192" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3192">
+        <v>4157185</v>
+      </c>
+      <c r="B3192" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3193" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3193">
+        <v>4303170</v>
+      </c>
+      <c r="B3193" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3194" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3194">
+        <v>4303171</v>
+      </c>
+      <c r="B3194" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3195" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3195">
+        <v>4222946</v>
+      </c>
+      <c r="B3195" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3196" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3196">
+        <v>4303181</v>
+      </c>
+      <c r="B3196" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3197" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3197">
+        <v>4303182</v>
+      </c>
+      <c r="B3197" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 30.10.2025 part 1
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4714DD03-DD1B-A84D-8AFF-DAD97F007B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA535D9-03A0-7940-98C9-48DFC2B80F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="6840" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9840" yWindow="6540" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +149,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -255,7 +255,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3197"/>
+  <dimension ref="A1:B3203"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3194" sqref="E3194"/>
+      <selection activeCell="D3200" sqref="D3200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25986,6 +25986,54 @@
         <v>4303182</v>
       </c>
       <c r="B3197" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3198" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3198">
+        <v>4390133</v>
+      </c>
+      <c r="B3198" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3199" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3199">
+        <v>4390134</v>
+      </c>
+      <c r="B3199" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3200" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3200">
+        <v>4390160</v>
+      </c>
+      <c r="B3200" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3201" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3201">
+        <v>4390161</v>
+      </c>
+      <c r="B3201" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3202" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3202">
+        <v>4390167</v>
+      </c>
+      <c r="B3202" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3203" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3203">
+        <v>4390168</v>
+      </c>
+      <c r="B3203" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 30.10.2025 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA535D9-03A0-7940-98C9-48DFC2B80F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7855AA85-E4ED-5C4C-9A90-259FDD731317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9840" yWindow="6540" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3203"/>
+  <dimension ref="A1:B3202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3200" sqref="D3200"/>
+      <selection activeCell="J3192" sqref="J3192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26027,14 +26027,6 @@
       </c>
       <c r="B3202" s="3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="3203" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3203">
-        <v>4390168</v>
-      </c>
-      <c r="B3203" s="3">
-        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ozon fixes 30.10.2025 part 4
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7855AA85-E4ED-5C4C-9A90-259FDD731317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3C896F-0256-BB43-9CC6-892047794D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9840" yWindow="6540" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3202"/>
+  <dimension ref="A1:B3206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J3192" sqref="J3192"/>
+      <selection activeCell="C3208" sqref="C3208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26027,6 +26027,38 @@
       </c>
       <c r="B3202" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3203" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3203">
+        <v>4300077</v>
+      </c>
+      <c r="B3203" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3204" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3204">
+        <v>4311320</v>
+      </c>
+      <c r="B3204" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3205" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3205">
+        <v>4319850</v>
+      </c>
+      <c r="B3205" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3206" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3206">
+        <v>4335413</v>
+      </c>
+      <c r="B3206" s="3">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ozon fixes 13.11.2025 part 1
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D6500C-93D8-8A4A-829D-D05C8F8B95C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB542DE-65C0-2848-80B8-EBE71F84A27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9840" yWindow="6520" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3217"/>
+  <dimension ref="A1:B3218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3186" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3195" sqref="G3195"/>
+      <selection activeCell="B3221" sqref="B3221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26146,6 +26146,14 @@
         <v>4501211</v>
       </c>
       <c r="B3217" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3218" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3218">
+        <v>4488310</v>
+      </c>
+      <c r="B3218" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 18.11.25 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB542DE-65C0-2848-80B8-EBE71F84A27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD6B27-6A22-5643-AAC1-F5250B9AAD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9840" yWindow="6520" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +149,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -255,7 +255,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3218"/>
+  <dimension ref="A1:B3224"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3186" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3221" sqref="B3221"/>
+      <selection activeCell="B3222" sqref="B3222:B3224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26154,6 +26154,54 @@
         <v>4488310</v>
       </c>
       <c r="B3218" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3219" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3219">
+        <v>4300034</v>
+      </c>
+      <c r="B3219" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3220" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3220">
+        <v>4390167</v>
+      </c>
+      <c r="B3220" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3221" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3221">
+        <v>4534287</v>
+      </c>
+      <c r="B3221" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3222" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3222">
+        <v>4400437</v>
+      </c>
+      <c r="B3222" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3223" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3223">
+        <v>4534299</v>
+      </c>
+      <c r="B3223" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3224" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3224">
+        <v>4534300</v>
+      </c>
+      <c r="B3224" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 01.12.2025 part 1
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBD6B27-6A22-5643-AAC1-F5250B9AAD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5ED2F0-E6A3-9C4B-BEB3-DA4A2650CA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="6520" windowWidth="23640" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16820" yWindow="680" windowWidth="19640" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3224"/>
+  <dimension ref="A1:B3254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3186" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3222" sqref="B3222:B3224"/>
+    <sheetView tabSelected="1" topLeftCell="A3207" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3255" sqref="A3255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26203,6 +26203,246 @@
       </c>
       <c r="B3224" s="3">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="3225" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3225">
+        <v>4400467</v>
+      </c>
+      <c r="B3225" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3226" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3226">
+        <v>4628617</v>
+      </c>
+      <c r="B3226" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3227" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3227">
+        <v>4628618</v>
+      </c>
+      <c r="B3227" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3228" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3228">
+        <v>4387203</v>
+      </c>
+      <c r="B3228" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3229" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3229">
+        <v>4628642</v>
+      </c>
+      <c r="B3229" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3230" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3230">
+        <v>4628643</v>
+      </c>
+      <c r="B3230" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3231" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3231">
+        <v>4386136</v>
+      </c>
+      <c r="B3231" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3232" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3232">
+        <v>4628650</v>
+      </c>
+      <c r="B3232" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3233" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3233">
+        <v>4628651</v>
+      </c>
+      <c r="B3233" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3234" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3234">
+        <v>4373574</v>
+      </c>
+      <c r="B3234" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3235" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3235">
+        <v>4628667</v>
+      </c>
+      <c r="B3235" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3236" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3236">
+        <v>4628668</v>
+      </c>
+      <c r="B3236" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3237" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3237">
+        <v>4367560</v>
+      </c>
+      <c r="B3237" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3238" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3238">
+        <v>4628685</v>
+      </c>
+      <c r="B3238" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3239" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3239">
+        <v>4628686</v>
+      </c>
+      <c r="B3239" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3240" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3240">
+        <v>4364283</v>
+      </c>
+      <c r="B3240" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3241" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3241">
+        <v>4628692</v>
+      </c>
+      <c r="B3241" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3242" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3242">
+        <v>4628693</v>
+      </c>
+      <c r="B3242" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3243" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3243">
+        <v>4355380</v>
+      </c>
+      <c r="B3243" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3244" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3244">
+        <v>4628701</v>
+      </c>
+      <c r="B3244" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3245" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3245">
+        <v>4628702</v>
+      </c>
+      <c r="B3245" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3246" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3246">
+        <v>4347126</v>
+      </c>
+      <c r="B3246" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3247" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3247">
+        <v>4628713</v>
+      </c>
+      <c r="B3247" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3248" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3248">
+        <v>4628714</v>
+      </c>
+      <c r="B3248" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3249" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3249">
+        <v>4341330</v>
+      </c>
+      <c r="B3249" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3250" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3250">
+        <v>4628718</v>
+      </c>
+      <c r="B3250" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3251" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3251">
+        <v>4628719</v>
+      </c>
+      <c r="B3251" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3252" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3252">
+        <v>4330873</v>
+      </c>
+      <c r="B3252" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3253" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3253">
+        <v>4628732</v>
+      </c>
+      <c r="B3253" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3254" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3254">
+        <v>4628733</v>
+      </c>
+      <c r="B3254" s="3">
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ozon fixes 01.12.2025 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5ED2F0-E6A3-9C4B-BEB3-DA4A2650CA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A5F3A4-B2D0-1648-9585-9C37FF743B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16820" yWindow="680" windowWidth="19640" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3254"/>
+  <dimension ref="A1:B3260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3207" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3255" sqref="A3255"/>
+      <selection activeCell="A3259" sqref="A3259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26443,6 +26443,54 @@
       </c>
       <c r="B3254" s="3">
         <v>10.5</v>
+      </c>
+    </row>
+    <row r="3255" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3255">
+        <v>4489353</v>
+      </c>
+      <c r="B3255" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3256" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3256">
+        <v>4556688</v>
+      </c>
+      <c r="B3256" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3257" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3257">
+        <v>4375547</v>
+      </c>
+      <c r="B3257" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3258" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3258">
+        <v>4454993</v>
+      </c>
+      <c r="B3258" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3259" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3259">
+        <v>4510727</v>
+      </c>
+      <c r="B3259" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3260" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3260">
+        <v>4629072</v>
+      </c>
+      <c r="B3260" s="3">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ozon fixes 26.12.2025 part 1
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A5F3A4-B2D0-1648-9585-9C37FF743B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FF49AB-2D7D-8041-ADE9-D6B11FA1125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="680" windowWidth="19640" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14920" yWindow="680" windowWidth="19640" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3260"/>
+  <dimension ref="A1:B3268"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3207" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3259" sqref="A3259"/>
+      <selection activeCell="B3267" sqref="B3267:B3268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26490,6 +26490,70 @@
         <v>4629072</v>
       </c>
       <c r="B3260" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3261" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3261">
+        <v>4832239</v>
+      </c>
+      <c r="B3261" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3262" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3262">
+        <v>4832240</v>
+      </c>
+      <c r="B3262" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3263" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3263">
+        <v>4832305</v>
+      </c>
+      <c r="B3263" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3264" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3264">
+        <v>4832306</v>
+      </c>
+      <c r="B3264" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3265" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3265">
+        <v>4832345</v>
+      </c>
+      <c r="B3265" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3266" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3266">
+        <v>4832346</v>
+      </c>
+      <c r="B3266" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3267" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3267">
+        <v>4832374</v>
+      </c>
+      <c r="B3267" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3268" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3268">
+        <v>4832375</v>
+      </c>
+      <c r="B3268" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 26.12.2025 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FF49AB-2D7D-8041-ADE9-D6B11FA1125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FB57C-BD82-8145-A1FD-71BC352C36CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14920" yWindow="680" windowWidth="19640" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16820" yWindow="680" windowWidth="17740" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3268"/>
+  <dimension ref="A1:B3274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3207" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3267" sqref="B3267:B3268"/>
+    <sheetView tabSelected="1" topLeftCell="A3216" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3273" sqref="B3273:B3274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26554,6 +26554,54 @@
         <v>4832375</v>
       </c>
       <c r="B3268" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3269" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3269">
+        <v>4832436</v>
+      </c>
+      <c r="B3269" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3270" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3270">
+        <v>4832437</v>
+      </c>
+      <c r="B3270" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3271" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3271">
+        <v>4832501</v>
+      </c>
+      <c r="B3271" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3272" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3272">
+        <v>4832502</v>
+      </c>
+      <c r="B3272" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3273" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3273">
+        <v>4832552</v>
+      </c>
+      <c r="B3273" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3274" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3274">
+        <v>4832553</v>
+      </c>
+      <c r="B3274" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 26.12.2025 part 4
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62FB57C-BD82-8145-A1FD-71BC352C36CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35C0535-6720-A047-ADD1-3365621E5F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16820" yWindow="680" windowWidth="17740" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3274"/>
+  <dimension ref="A1:B3323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3216" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3273" sqref="B3273:B3274"/>
+    <sheetView tabSelected="1" topLeftCell="A3289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3323" sqref="B3323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26602,6 +26602,398 @@
         <v>4832553</v>
       </c>
       <c r="B3274" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3275" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3275">
+        <v>4833319</v>
+      </c>
+      <c r="B3275" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3276" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3276">
+        <v>4833320</v>
+      </c>
+      <c r="B3276" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3277" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3277">
+        <v>4833401</v>
+      </c>
+      <c r="B3277" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3278" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3278">
+        <v>4833402</v>
+      </c>
+      <c r="B3278" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3279" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3279">
+        <v>4833547</v>
+      </c>
+      <c r="B3279" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3280" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3280">
+        <v>4833548</v>
+      </c>
+      <c r="B3280" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3281" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3281">
+        <v>4833549</v>
+      </c>
+      <c r="B3281" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3282" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3282">
+        <v>4833550</v>
+      </c>
+      <c r="B3282" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3283" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3283">
+        <v>4833545</v>
+      </c>
+      <c r="B3283" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3284" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3284">
+        <v>4833546</v>
+      </c>
+      <c r="B3284" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3285" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3285">
+        <v>4833541</v>
+      </c>
+      <c r="B3285" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3286" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3286">
+        <v>4833542</v>
+      </c>
+      <c r="B3286" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3287" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3287">
+        <v>4833537</v>
+      </c>
+      <c r="B3287" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3288" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3288">
+        <v>4833538</v>
+      </c>
+      <c r="B3288" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3289" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3289">
+        <v>4833539</v>
+      </c>
+      <c r="B3289" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3290" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3290">
+        <v>4833540</v>
+      </c>
+      <c r="B3290" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3291" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3291">
+        <v>4833543</v>
+      </c>
+      <c r="B3291" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3292" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3292">
+        <v>4833544</v>
+      </c>
+      <c r="B3292" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3293" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3293">
+        <v>4833535</v>
+      </c>
+      <c r="B3293" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3294" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3294">
+        <v>4833536</v>
+      </c>
+      <c r="B3294" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3295" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3295">
+        <v>4833533</v>
+      </c>
+      <c r="B3295" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3296" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3296">
+        <v>4833534</v>
+      </c>
+      <c r="B3296" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3297" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3297">
+        <v>4833531</v>
+      </c>
+      <c r="B3297" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3298" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3298">
+        <v>4833532</v>
+      </c>
+      <c r="B3298" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3299" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3299">
+        <v>4833529</v>
+      </c>
+      <c r="B3299" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3300" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3300">
+        <v>4833530</v>
+      </c>
+      <c r="B3300" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3301" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3301">
+        <v>4833527</v>
+      </c>
+      <c r="B3301" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3302" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3302">
+        <v>4833528</v>
+      </c>
+      <c r="B3302" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3303" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3303">
+        <v>4833525</v>
+      </c>
+      <c r="B3303" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3304" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3304">
+        <v>4833526</v>
+      </c>
+      <c r="B3304" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3305" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3305">
+        <v>4833523</v>
+      </c>
+      <c r="B3305" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3306" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3306">
+        <v>4833524</v>
+      </c>
+      <c r="B3306" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3307" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3307">
+        <v>4833521</v>
+      </c>
+      <c r="B3307" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3308" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3308">
+        <v>4833522</v>
+      </c>
+      <c r="B3308" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3309" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3309">
+        <v>4833519</v>
+      </c>
+      <c r="B3309" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3310" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3310">
+        <v>4833520</v>
+      </c>
+      <c r="B3310" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3311" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3311">
+        <v>4833517</v>
+      </c>
+      <c r="B3311" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3312" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3312">
+        <v>4833518</v>
+      </c>
+      <c r="B3312" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3313" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3313">
+        <v>4833515</v>
+      </c>
+      <c r="B3313" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3314" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3314">
+        <v>4833516</v>
+      </c>
+      <c r="B3314" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3315" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3315">
+        <v>4833513</v>
+      </c>
+      <c r="B3315" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3316" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3316">
+        <v>4833514</v>
+      </c>
+      <c r="B3316" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3317" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3317">
+        <v>4833511</v>
+      </c>
+      <c r="B3317" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3318" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3318">
+        <v>4833512</v>
+      </c>
+      <c r="B3318" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3319" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3319">
+        <v>4833505</v>
+      </c>
+      <c r="B3319" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3320" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3320">
+        <v>4833506</v>
+      </c>
+      <c r="B3320" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3321" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3321">
+        <v>4833507</v>
+      </c>
+      <c r="B3321" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3322" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3322">
+        <v>4833508</v>
+      </c>
+      <c r="B3322" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3323" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3323">
+        <v>4833510</v>
+      </c>
+      <c r="B3323" s="3">
         <v>3.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 15.01.2026 part 2
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35C0535-6720-A047-ADD1-3365621E5F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF43B9-72D0-0C46-9CD8-BE8452A561AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16820" yWindow="680" windowWidth="17740" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3323"/>
+  <dimension ref="A1:B3341"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3323" sqref="B3323"/>
+      <selection activeCell="B3340" sqref="B3340:B3341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26995,6 +26995,150 @@
       </c>
       <c r="B3323" s="3">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="3324" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3324">
+        <v>4976994</v>
+      </c>
+      <c r="B3324" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3325" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3325">
+        <v>4976995</v>
+      </c>
+      <c r="B3325" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3326" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3326">
+        <v>4977008</v>
+      </c>
+      <c r="B3326" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3327" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3327">
+        <v>4977009</v>
+      </c>
+      <c r="B3327" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3328" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3328">
+        <v>4977044</v>
+      </c>
+      <c r="B3328" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3329" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3329">
+        <v>4977045</v>
+      </c>
+      <c r="B3329" s="3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="3330" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3330">
+        <v>4977074</v>
+      </c>
+      <c r="B3330" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3331" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3331">
+        <v>4977075</v>
+      </c>
+      <c r="B3331" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3332" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3332">
+        <v>4977115</v>
+      </c>
+      <c r="B3332" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3333" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3333">
+        <v>4977116</v>
+      </c>
+      <c r="B3333" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3334" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3334">
+        <v>4977132</v>
+      </c>
+      <c r="B3334" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3335" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3335">
+        <v>4977133</v>
+      </c>
+      <c r="B3335" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3336" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3336">
+        <v>4977148</v>
+      </c>
+      <c r="B3336" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3337" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3337">
+        <v>4977149</v>
+      </c>
+      <c r="B3337" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3338" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3338">
+        <v>4977175</v>
+      </c>
+      <c r="B3338" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3339" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3339">
+        <v>4977176</v>
+      </c>
+      <c r="B3339" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3340" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3340">
+        <v>4977191</v>
+      </c>
+      <c r="B3340" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3341" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3341">
+        <v>4977192</v>
+      </c>
+      <c r="B3341" s="3">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ozon fixes 15.01.2026 part 5
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDF43B9-72D0-0C46-9CD8-BE8452A561AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FCB146-2801-5E47-8C71-1F1471FD998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16820" yWindow="680" windowWidth="17740" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3341"/>
+  <dimension ref="A1:B3345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3340" sqref="B3340:B3341"/>
+      <selection activeCell="B3344" sqref="B3344:B3345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27138,6 +27138,38 @@
         <v>4977192</v>
       </c>
       <c r="B3341" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3342" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3342">
+        <v>4977336</v>
+      </c>
+      <c r="B3342" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3343" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3343">
+        <v>4977337</v>
+      </c>
+      <c r="B3343" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3344" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3344">
+        <v>4977349</v>
+      </c>
+      <c r="B3344" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3345" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3345">
+        <v>4977350</v>
+      </c>
+      <c r="B3345" s="3">
         <v>7.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ozon fixes 29.01.2026 part 1
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FCB146-2801-5E47-8C71-1F1471FD998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313B54DA-0CE6-CF40-9B50-B3DFC13647B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16820" yWindow="680" windowWidth="17740" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3345"/>
+  <dimension ref="A1:B3348"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3344" sqref="B3344:B3345"/>
+      <selection activeCell="B3348" sqref="B3348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27170,6 +27170,30 @@
         <v>4977350</v>
       </c>
       <c r="B3345" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3346" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3346">
+        <v>5085248</v>
+      </c>
+      <c r="B3346" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3347" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3347">
+        <v>5085292</v>
+      </c>
+      <c r="B3347" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3348" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3348">
+        <v>5085299</v>
+      </c>
+      <c r="B3348" s="3">
         <v>7.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes part 1 17.02.2026
</commit_message>
<xml_diff>
--- a/c_co.xlsx
+++ b/c_co.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313B54DA-0CE6-CF40-9B50-B3DFC13647B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2755FC5-9B2E-E346-AD53-6B2D1CDE6DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="680" windowWidth="17740" windowHeight="19820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16820" yWindow="660" windowWidth="17740" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3348"/>
+  <dimension ref="A1:B3349"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3348" sqref="B3348"/>
+      <selection activeCell="D3348" sqref="D3348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27195,6 +27195,14 @@
       </c>
       <c r="B3348" s="3">
         <v>7.5</v>
+      </c>
+    </row>
+    <row r="3349" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3349">
+        <v>5239620</v>
+      </c>
+      <c r="B3349" s="3">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>